<commit_message>
Modified patho figures with bacillus data
</commit_message>
<xml_diff>
--- a/Volatile.xlsx
+++ b/Volatile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Lab/Serratia/Volatiles_Rmd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3437FF1-7A7B-584A-989B-CC7B88214D3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55644BE-F348-B749-B67F-DD24D62B33BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31620" yWindow="-11540" windowWidth="25200" windowHeight="14180" firstSheet="9" activeTab="16" xr2:uid="{5ADA3297-C869-F041-ABCD-259B162EE42B}"/>
+    <workbookView xWindow="-22480" yWindow="-6320" windowWidth="28800" windowHeight="17540" activeTab="7" xr2:uid="{5ADA3297-C869-F041-ABCD-259B162EE42B}"/>
   </bookViews>
   <sheets>
     <sheet name="Serratia Multistrain Analysis" sheetId="7" r:id="rId1"/>
@@ -32,9 +32,6 @@
     <sheet name="refs" sheetId="34" r:id="rId17"/>
     <sheet name="Strawberry" sheetId="11" r:id="rId18"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId19"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">RSI_Over85!$E$1:$G$2707</definedName>
     <definedName name="_xlnm.Extract" localSheetId="12">RSI_Over85!$E:$G</definedName>
@@ -55,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11075" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11093" uniqueCount="854">
   <si>
     <t>Nothing</t>
   </si>
@@ -2626,12 +2623,15 @@
   <si>
     <t>Batrachochytrium dendrobatidis, Batrachochytrium salamandrivorans, Candida albicans, Diaphorina citri, Didymella applanata, Lasiodiplodia theobromae, Pythium ultimum, Phytophthora parasitica, Phytophthora cinnamomi, Phytophthora citrophora, Saccharomyces cerevisiae, Curvularia eragrostidis, Pestalotiopsis theae, Colletotrichum camelliae, Lasiodiplodia theobromae,  Rhizoctonia solani</t>
   </si>
+  <si>
+    <t>B. subtilis E9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2685,6 +2685,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2707,7 +2714,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2724,6 +2731,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
@@ -2743,350 +2751,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Spent_Media"/>
-      <sheetName val="UV Death"/>
-      <sheetName val="UV_mutants_2-und"/>
-      <sheetName val="EC50"/>
-      <sheetName val="Nc 2-und"/>
-      <sheetName val="OD"/>
-      <sheetName val="Sm Vs Zygos"/>
-      <sheetName val="Dil_VOC_RS_24"/>
-      <sheetName val="FGSC_2489_V_All"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>18 Hours 2-undecanone</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>18 Hours No 2-undecanone</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>24 Hours 2-undecanone</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>24 Hours No 2-undecanone</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>WTA</v>
-          </cell>
-          <cell r="B2">
-            <v>0.52</v>
-          </cell>
-          <cell r="C2">
-            <v>1.22</v>
-          </cell>
-          <cell r="D2">
-            <v>1.9</v>
-          </cell>
-          <cell r="E2">
-            <v>2.9</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>gna1*</v>
-          </cell>
-          <cell r="B3">
-            <v>0.52</v>
-          </cell>
-          <cell r="C3">
-            <v>0.64</v>
-          </cell>
-          <cell r="D3">
-            <v>1.9</v>
-          </cell>
-          <cell r="E3">
-            <v>2.9</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>gna1</v>
-          </cell>
-          <cell r="B4">
-            <v>0.5</v>
-          </cell>
-          <cell r="C4">
-            <v>0.5</v>
-          </cell>
-          <cell r="D4">
-            <v>1.92</v>
-          </cell>
-          <cell r="E4">
-            <v>2.9</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>gna2</v>
-          </cell>
-          <cell r="B5">
-            <v>0.4</v>
-          </cell>
-          <cell r="C5">
-            <v>0.54</v>
-          </cell>
-          <cell r="D5">
-            <v>2.12</v>
-          </cell>
-          <cell r="E5">
-            <v>2.9</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>gna2*</v>
-          </cell>
-          <cell r="B6">
-            <v>0.5</v>
-          </cell>
-          <cell r="C6">
-            <v>1.08</v>
-          </cell>
-          <cell r="D6">
-            <v>2.12</v>
-          </cell>
-          <cell r="E6">
-            <v>2.9</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>gna3</v>
-          </cell>
-          <cell r="B7">
-            <v>0.5</v>
-          </cell>
-          <cell r="C7">
-            <v>0.5</v>
-          </cell>
-          <cell r="D7">
-            <v>2.2000000000000002</v>
-          </cell>
-          <cell r="E7">
-            <v>2.9</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>gnb1</v>
-          </cell>
-          <cell r="B8">
-            <v>0.42</v>
-          </cell>
-          <cell r="C8">
-            <v>0.64</v>
-          </cell>
-          <cell r="D8">
-            <v>2.1</v>
-          </cell>
-          <cell r="E8">
-            <v>2.82</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>gng1</v>
-          </cell>
-          <cell r="B9">
-            <v>0.56000000000000005</v>
-          </cell>
-          <cell r="C9">
-            <v>0.88</v>
-          </cell>
-          <cell r="D9">
-            <v>1.86</v>
-          </cell>
-          <cell r="E9">
-            <v>2.78</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>cpc2</v>
-          </cell>
-          <cell r="B10">
-            <v>0.52</v>
-          </cell>
-          <cell r="C10">
-            <v>0.54</v>
-          </cell>
-          <cell r="D10">
-            <v>1.6</v>
-          </cell>
-          <cell r="E10">
-            <v>2.74</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>4.4721359549999999E-2</v>
-          </cell>
-          <cell r="C13">
-            <v>0.1095445115</v>
-          </cell>
-          <cell r="D13">
-            <v>0.39370039369999998</v>
-          </cell>
-          <cell r="E13">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>4.4721359549999999E-2</v>
-          </cell>
-          <cell r="C14">
-            <v>0.1140175425</v>
-          </cell>
-          <cell r="D14">
-            <v>0.39370039369999998</v>
-          </cell>
-          <cell r="E14">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>0</v>
-          </cell>
-          <cell r="C15">
-            <v>0</v>
-          </cell>
-          <cell r="D15">
-            <v>0.43243496619999999</v>
-          </cell>
-          <cell r="E15">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>0</v>
-          </cell>
-          <cell r="C16">
-            <v>5.4772255749999998E-2</v>
-          </cell>
-          <cell r="D16">
-            <v>0.42071367939999998</v>
-          </cell>
-          <cell r="E16">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>0</v>
-          </cell>
-          <cell r="C17">
-            <v>8.3666002650000001E-2</v>
-          </cell>
-          <cell r="D17">
-            <v>0.42071367939999998</v>
-          </cell>
-          <cell r="E17">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>0</v>
-          </cell>
-          <cell r="C18">
-            <v>0.1</v>
-          </cell>
-          <cell r="D18">
-            <v>0.32403703490000002</v>
-          </cell>
-          <cell r="E18">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>4.4721359549999999E-2</v>
-          </cell>
-          <cell r="C19">
-            <v>8.9442719099999998E-2</v>
-          </cell>
-          <cell r="D19">
-            <v>0.45276925690000003</v>
-          </cell>
-          <cell r="E19">
-            <v>0.1788854382</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>5.4772255749999998E-2</v>
-          </cell>
-          <cell r="C20">
-            <v>8.3666002650000001E-2</v>
-          </cell>
-          <cell r="D20">
-            <v>0.43931765270000001</v>
-          </cell>
-          <cell r="E20">
-            <v>0.1788854382</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>8.3666002650000001E-2</v>
-          </cell>
-          <cell r="C21">
-            <v>5.4772255749999998E-2</v>
-          </cell>
-          <cell r="D21">
-            <v>0.33911649919999998</v>
-          </cell>
-          <cell r="E21">
-            <v>0.1673320053</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>Pombe v 2-undecanone</v>
-          </cell>
-          <cell r="B24" t="str">
-            <v>Pombe No 2-undecanone</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>1.2E-2</v>
-          </cell>
-          <cell r="B25">
-            <v>0.74433333329999996</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>3.464101615E-3</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -91840,17 +91504,17 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -91868,17 +91532,17 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -91899,7 +91563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC72D4D4-1413-474D-B010-36E3964F1F48}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -92015,14 +91679,14 @@
       <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="16"/>
+      <c r="C16" s="17"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="16"/>
+      <c r="C17" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -92186,10 +91850,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19ADFF52-8F1C-4D96-9903-6C31EE3B3FFE}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -92225,14 +91889,14 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>300</v>
+        <v>835</v>
       </c>
       <c r="B2">
         <f>H2/57*100</f>
-        <v>8.7719298245614024</v>
+        <v>17.543859649122805</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:D10" si="0">I2/57*100</f>
+        <f t="shared" ref="C2:D13" si="0">I2/57*100</f>
         <v>61.403508771929829</v>
       </c>
       <c r="D2">
@@ -92243,7 +91907,7 @@
         <v>300</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I2">
         <v>35</v>
@@ -92257,11 +91921,11 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>300</v>
+        <v>835</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B10" si="1">H3/57*100</f>
-        <v>8.7719298245614024</v>
+        <f t="shared" ref="B3:B13" si="1">H3/57*100</f>
+        <v>17.543859649122805</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
@@ -92275,7 +91939,7 @@
         <v>300</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I3">
         <v>33</v>
@@ -92289,11 +91953,11 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>300</v>
+        <v>835</v>
       </c>
       <c r="B4">
         <f t="shared" si="1"/>
-        <v>8.7719298245614024</v>
+        <v>17.543859649122805</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
@@ -92307,7 +91971,7 @@
         <v>300</v>
       </c>
       <c r="H4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I4">
         <v>31</v>
@@ -92325,27 +91989,27 @@
       </c>
       <c r="B5">
         <f t="shared" si="1"/>
-        <v>8.7719298245614024</v>
+        <v>17.543859649122805</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>42.105263157894733</v>
+        <v>52.631578947368418</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>77.192982456140342</v>
+        <v>80.701754385964904</v>
       </c>
       <c r="G5" t="s">
         <v>298</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I5" s="1">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J5">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K5">
         <v>57</v>
@@ -92357,7 +92021,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="1"/>
-        <v>8.7719298245614024</v>
+        <v>17.543859649122805</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -92365,19 +92029,19 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>85.964912280701753</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
         <v>298</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I6" s="1">
         <v>29</v>
       </c>
       <c r="J6">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="K6">
         <v>57</v>
@@ -92389,27 +92053,27 @@
       </c>
       <c r="B7">
         <f t="shared" si="1"/>
-        <v>8.7719298245614024</v>
+        <v>17.543859649122805</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>45.614035087719294</v>
+        <v>54.385964912280706</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>73.68421052631578</v>
+        <v>84.210526315789465</v>
       </c>
       <c r="G7" t="s">
         <v>298</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I7" s="1">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J7">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="K7">
         <v>57</v>
@@ -92417,11 +92081,11 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>299</v>
+        <v>844</v>
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>8.7719298245614024</v>
+        <v>17.543859649122805</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -92435,7 +92099,7 @@
         <v>299</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I8" s="1">
         <v>29</v>
@@ -92449,11 +92113,11 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>299</v>
+        <v>844</v>
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
-        <v>8.7719298245614024</v>
+        <v>17.543859649122805</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -92467,7 +92131,7 @@
         <v>299</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I9" s="1">
         <v>27</v>
@@ -92481,11 +92145,11 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>299</v>
+        <v>844</v>
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>8.7719298245614024</v>
+        <v>17.543859649122805</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -92499,7 +92163,7 @@
         <v>299</v>
       </c>
       <c r="H10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I10" s="1">
         <v>32</v>
@@ -92508,6 +92172,102 @@
         <v>52</v>
       </c>
       <c r="K10">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>825</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>17.543859649122805</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>56.140350877192979</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G11" t="s">
+        <v>853</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11" s="1">
+        <v>32</v>
+      </c>
+      <c r="J11">
+        <v>57</v>
+      </c>
+      <c r="K11">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>825</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>17.543859649122805</v>
+      </c>
+      <c r="C12">
+        <f>I12/57*100</f>
+        <v>59.649122807017541</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>89.473684210526315</v>
+      </c>
+      <c r="G12" t="s">
+        <v>853</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1">
+        <v>34</v>
+      </c>
+      <c r="J12">
+        <v>51</v>
+      </c>
+      <c r="K12">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>825</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>17.543859649122805</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>52.631578947368418</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>89.473684210526315</v>
+      </c>
+      <c r="G13" t="s">
+        <v>853</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13" s="1">
+        <v>30</v>
+      </c>
+      <c r="J13">
+        <v>51</v>
+      </c>
+      <c r="K13">
         <v>57</v>
       </c>
     </row>
@@ -92673,10 +92433,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870191F1-71E4-41A1-80C7-FB5FD0648ABE}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D10"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -92712,14 +92472,14 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>300</v>
+        <v>835</v>
       </c>
       <c r="B2">
         <f>H2/57*100</f>
         <v>17.543859649122805</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:D10" si="0">I2/57*100</f>
+        <f t="shared" ref="C2:D13" si="0">I2/57*100</f>
         <v>33.333333333333329</v>
       </c>
       <c r="D2">
@@ -92741,10 +92501,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>300</v>
+        <v>835</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B10" si="1">H3/57*100</f>
+        <f t="shared" ref="B3:B13" si="1">H3/57*100</f>
         <v>17.543859649122805</v>
       </c>
       <c r="C3">
@@ -92770,7 +92530,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>300</v>
+        <v>835</v>
       </c>
       <c r="B4">
         <f t="shared" si="1"/>
@@ -92807,11 +92567,11 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>36.84210526315789</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>66.666666666666657</v>
+        <v>70.175438596491219</v>
       </c>
       <c r="G5" t="s">
         <v>298</v>
@@ -92820,10 +92580,10 @@
         <v>10</v>
       </c>
       <c r="I5">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J5">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K5">
         <v>48</v>
@@ -92839,11 +92599,11 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>28.07017543859649</v>
+        <v>38.596491228070171</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>64.912280701754383</v>
+        <v>70.175438596491219</v>
       </c>
       <c r="G6" t="s">
         <v>298</v>
@@ -92852,10 +92612,10 @@
         <v>10</v>
       </c>
       <c r="I6">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="J6">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K6">
         <v>47</v>
@@ -92871,11 +92631,11 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>33.333333333333329</v>
+        <v>42.105263157894733</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>59.649122807017541</v>
+        <v>70.175438596491219</v>
       </c>
       <c r="G7" t="s">
         <v>298</v>
@@ -92884,10 +92644,10 @@
         <v>10</v>
       </c>
       <c r="I7">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J7">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="K7">
         <v>50</v>
@@ -92895,7 +92655,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>299</v>
+        <v>844</v>
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
@@ -92927,7 +92687,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>299</v>
+        <v>844</v>
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
@@ -92959,7 +92719,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>299</v>
+        <v>844</v>
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
@@ -92987,6 +92747,93 @@
       </c>
       <c r="K10">
         <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>825</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>17.543859649122805</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>52.631578947368418</v>
+      </c>
+      <c r="G11" t="s">
+        <v>853</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>19</v>
+      </c>
+      <c r="J11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>825</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>17.543859649122805</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>38.596491228070171</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>56.140350877192979</v>
+      </c>
+      <c r="G12" t="s">
+        <v>853</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>22</v>
+      </c>
+      <c r="J12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>825</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>17.543859649122805</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>42.105263157894733</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>61.403508771929829</v>
+      </c>
+      <c r="G13" t="s">
+        <v>853</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>24</v>
+      </c>
+      <c r="J13">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -92996,10 +92843,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80649262-E98F-4B85-B9EE-B514DB2846D7}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D10"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -93035,21 +92882,21 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>300</v>
+        <v>835</v>
       </c>
       <c r="B2">
         <f>I2/57*100</f>
         <v>17.543859649122805</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:D10" si="0">J2/57*100</f>
+        <f t="shared" ref="C2:D13" si="0">J2/57*100</f>
         <v>35.087719298245609</v>
       </c>
       <c r="D2">
         <f t="shared" si="0"/>
         <v>75.438596491228068</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="14" t="s">
         <v>300</v>
       </c>
       <c r="I2">
@@ -93067,10 +92914,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>300</v>
+        <v>835</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B10" si="1">I3/57*100</f>
+        <f t="shared" ref="B3:B13" si="1">I3/57*100</f>
         <v>17.543859649122805</v>
       </c>
       <c r="C3">
@@ -93081,7 +92928,7 @@
         <f t="shared" si="0"/>
         <v>80.701754385964904</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="14" t="s">
         <v>300</v>
       </c>
       <c r="I3">
@@ -93099,7 +92946,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>300</v>
+        <v>835</v>
       </c>
       <c r="B4">
         <f t="shared" si="1"/>
@@ -93113,7 +92960,7 @@
         <f t="shared" si="0"/>
         <v>80.701754385964904</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="14" t="s">
         <v>300</v>
       </c>
       <c r="I4">
@@ -93145,7 +92992,7 @@
         <f t="shared" si="0"/>
         <v>64.912280701754383</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="14" t="s">
         <v>298</v>
       </c>
       <c r="I5">
@@ -93177,7 +93024,7 @@
         <f t="shared" si="0"/>
         <v>66.666666666666657</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="14" t="s">
         <v>298</v>
       </c>
       <c r="I6">
@@ -93209,7 +93056,7 @@
         <f t="shared" si="0"/>
         <v>73.68421052631578</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="14" t="s">
         <v>298</v>
       </c>
       <c r="I7">
@@ -93227,7 +93074,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>299</v>
+        <v>844</v>
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
@@ -93241,7 +93088,7 @@
         <f t="shared" si="0"/>
         <v>71.929824561403507</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="14" t="s">
         <v>299</v>
       </c>
       <c r="I8">
@@ -93259,7 +93106,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>299</v>
+        <v>844</v>
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
@@ -93273,7 +93120,7 @@
         <f t="shared" si="0"/>
         <v>73.68421052631578</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="14" t="s">
         <v>299</v>
       </c>
       <c r="I9">
@@ -93291,7 +93138,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>299</v>
+        <v>844</v>
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
@@ -93305,7 +93152,7 @@
         <f t="shared" si="0"/>
         <v>80.701754385964904</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="14" t="s">
         <v>299</v>
       </c>
       <c r="I10">
@@ -93319,6 +93166,93 @@
       </c>
       <c r="L10">
         <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>825</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>17.543859649122805</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>26.315789473684209</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>57.894736842105267</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>853</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>15</v>
+      </c>
+      <c r="K11">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>825</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>17.543859649122805</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>28.07017543859649</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>49.122807017543856</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>853</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>825</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>17.543859649122805</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>22.807017543859647</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>68.421052631578945</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>853</v>
+      </c>
+      <c r="I13">
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>13</v>
+      </c>
+      <c r="K13">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -93651,10 +93585,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AC6FFA-60E7-4252-9C27-30E0E9EA75FA}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:D16"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -94033,7 +93967,11 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>54.385964912280706</v>
+        <v>38.596491228070171</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>80.701754385964904</v>
       </c>
       <c r="H13" t="s">
         <v>297</v>
@@ -94042,7 +93980,10 @@
         <v>5</v>
       </c>
       <c r="J13">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="K13">
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -94055,7 +93996,11 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>56.140350877192979</v>
+        <v>45.614035087719294</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="H14" t="s">
         <v>297</v>
@@ -94064,7 +94009,10 @@
         <v>5</v>
       </c>
       <c r="J14">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="K14">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -94077,7 +94025,11 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>50.877192982456144</v>
+        <v>43.859649122807014</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="H15" t="s">
         <v>297</v>
@@ -94086,7 +94038,10 @@
         <v>5</v>
       </c>
       <c r="J15">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="K15">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -94099,7 +94054,11 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>52.631578947368418</v>
+        <v>40.350877192982452</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="H16" t="s">
         <v>297</v>
@@ -94108,7 +94067,44 @@
         <v>5</v>
       </c>
       <c r="J16">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="K16">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <f>TTEST(J5:J9,J19:J25,2,2)</f>
+        <v>1.3577665393918952E-4</v>
+      </c>
+      <c r="J19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -94120,8 +94116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E65D0FE-C98B-4764-9D9B-7818AB1C6AC6}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -94358,11 +94354,28 @@
         <f t="shared" si="1"/>
         <v>8.7719298245614024</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>80.701754385964904</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
       <c r="H8" t="s">
         <v>299</v>
       </c>
       <c r="I8">
         <v>5</v>
+      </c>
+      <c r="J8">
+        <v>46</v>
+      </c>
+      <c r="K8">
+        <v>57</v>
+      </c>
+      <c r="L8">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -94373,11 +94386,28 @@
         <f t="shared" si="1"/>
         <v>8.7719298245614024</v>
       </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
       <c r="H9" t="s">
         <v>299</v>
       </c>
       <c r="I9">
         <v>5</v>
+      </c>
+      <c r="J9">
+        <v>57</v>
+      </c>
+      <c r="K9">
+        <v>57</v>
+      </c>
+      <c r="L9">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -94388,11 +94418,28 @@
         <f t="shared" si="1"/>
         <v>8.7719298245614024</v>
       </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
       <c r="H10" t="s">
         <v>299</v>
       </c>
       <c r="I10">
         <v>5</v>
+      </c>
+      <c r="J10">
+        <v>57</v>
+      </c>
+      <c r="K10">
+        <v>57</v>
+      </c>
+      <c r="L10">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -94407,6 +94454,10 @@
         <f t="shared" si="0"/>
         <v>77.192982456140342</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
       <c r="H11" t="s">
         <v>297</v>
       </c>
@@ -94434,6 +94485,10 @@
       <c r="C12">
         <f t="shared" si="0"/>
         <v>91.228070175438589</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="H12" t="s">
         <v>297</v>

</xml_diff>